<commit_message>
add in data sources tab
</commit_message>
<xml_diff>
--- a/Data/18_FeSources/FeSources.xlsx
+++ b/Data/18_FeSources/FeSources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/hannah_cox_education_gov_uk/Documents/Documents/Projects/lsip_dashboard/Data/18_FeSources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/18_FeSources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0BDD28A-F030-4D21-AB82-F93368626CC3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="16920" windowHeight="10540" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Source</t>
   </si>
@@ -63,72 +63,6 @@
   </si>
   <si>
     <t>Apply for access here</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subnational indicators explorer </t>
-  </si>
-  <si>
-    <t>Association of Colleges (AoC)</t>
-  </si>
-  <si>
-    <t>https://www.ons.gov.uk/peoplepopulationandcommunity/wellbeing/articles/subnationalindicatorsexplorer/2022-01-06</t>
-  </si>
-  <si>
-    <t>https://www.aoc.co.uk/research-unit/data-sources</t>
-  </si>
-  <si>
-    <t>Census</t>
-  </si>
-  <si>
-    <t>https://census.gov.uk/local-authorities</t>
-  </si>
-  <si>
-    <t>NOMIS</t>
-  </si>
-  <si>
-    <t>Compare a local authority and the UK average (median) local authority by different indicators, such as weekly pay and healthy life expectancy.</t>
-  </si>
-  <si>
-    <t>Publicly available</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contains a range of topics including labour market and education by local authority. </t>
-  </si>
-  <si>
-    <t>ONS</t>
-  </si>
-  <si>
-    <t>Query labour market data at national, regional and local levels</t>
-  </si>
-  <si>
-    <t>https://www.nomisweb.co.uk/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publicly available, with more functionality if you create an account. </t>
-  </si>
-  <si>
-    <t>Explore Education Statistics</t>
-  </si>
-  <si>
-    <t>DfE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A range of educational data published by the Department of Education </t>
-  </si>
-  <si>
-    <t>https://explore-education-statistics.service.gov.uk/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publicly available </t>
-  </si>
-  <si>
-    <t>Lists useful data sources related to colleges</t>
-  </si>
-  <si>
-    <t>AoC</t>
-  </si>
-  <si>
-    <t>Working Futures 2035</t>
   </si>
 </sst>
 </file>
@@ -472,7 +406,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -480,22 +414,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455C0F38-06FA-4C4D-8065-41AFD4764DD8}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -512,7 +445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -524,96 +457,6 @@
       </c>
       <c r="E2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding FE sources table
</commit_message>
<xml_diff>
--- a/Data/18_FeSources/FeSources.xlsx
+++ b/Data/18_FeSources/FeSources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/18_FeSources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/sula_marshall_education_gov_uk/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B02DA01-9AE0-4AEA-BEBC-BFD7C87DF43C}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="16920" windowHeight="10540" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Source</t>
   </si>
@@ -63,6 +63,69 @@
   </si>
   <si>
     <t>Apply for access here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subnational indicators explorer </t>
+  </si>
+  <si>
+    <t>Association of Colleges (AoC)</t>
+  </si>
+  <si>
+    <t>https://www.ons.gov.uk/peoplepopulationandcommunity/wellbeing/articles/subnationalindicatorsexplorer/2022-01-06</t>
+  </si>
+  <si>
+    <t>https://www.aoc.co.uk/research-unit/data-sources</t>
+  </si>
+  <si>
+    <t>Census</t>
+  </si>
+  <si>
+    <t>https://census.gov.uk/local-authorities</t>
+  </si>
+  <si>
+    <t>NOMIS</t>
+  </si>
+  <si>
+    <t>Compare a local authority and the UK average (median) local authority by different indicators, such as weekly pay and healthy life expectancy.</t>
+  </si>
+  <si>
+    <t>Publicly available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains a range of topics including labour market and education by local authority. </t>
+  </si>
+  <si>
+    <t>ONS</t>
+  </si>
+  <si>
+    <t>Query labour market data at national, regional and local levels</t>
+  </si>
+  <si>
+    <t>https://www.nomisweb.co.uk/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publicly available, with more functionality if you create an account. </t>
+  </si>
+  <si>
+    <t>Explore Education Statistics</t>
+  </si>
+  <si>
+    <t>DfE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A range of educational data published by the Department of Education </t>
+  </si>
+  <si>
+    <t>https://explore-education-statistics.service.gov.uk/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publicly available </t>
+  </si>
+  <si>
+    <t>Lists useful data sources related to colleges</t>
+  </si>
+  <si>
+    <t>AoC</t>
   </si>
 </sst>
 </file>
@@ -406,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,21 +477,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455C0F38-06FA-4C4D-8065-41AFD4764DD8}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.07421875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.4609375" customWidth="1"/>
+    <col min="5" max="5" width="20.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -445,7 +509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -457,6 +521,91 @@
       </c>
       <c r="E2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add in data sources and time line fix the top of the page links
</commit_message>
<xml_diff>
--- a/Data/18_FeSources/FeSources.xlsx
+++ b/Data/18_FeSources/FeSources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/18_FeSources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/hannah_cox_education_gov_uk/Documents/Documents/Projects/lsip_dashboard/Data/18_FeSources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7297E987-FB5B-4F30-A6A2-190410A21B14}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="16920" windowHeight="10540" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
+    <workbookView minimized="1" xWindow="1065" yWindow="1185" windowWidth="5400" windowHeight="2813" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Source</t>
   </si>
@@ -63,6 +63,72 @@
   </si>
   <si>
     <t>Apply for access here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subnational indicators explorer </t>
+  </si>
+  <si>
+    <t>Association of Colleges (AoC)</t>
+  </si>
+  <si>
+    <t>https://www.ons.gov.uk/peoplepopulationandcommunity/wellbeing/articles/subnationalindicatorsexplorer/2022-01-06</t>
+  </si>
+  <si>
+    <t>https://www.aoc.co.uk/research-unit/data-sources</t>
+  </si>
+  <si>
+    <t>Census</t>
+  </si>
+  <si>
+    <t>https://census.gov.uk/local-authorities</t>
+  </si>
+  <si>
+    <t>NOMIS</t>
+  </si>
+  <si>
+    <t>Compare a local authority and the UK average (median) local authority by different indicators, such as weekly pay and healthy life expectancy.</t>
+  </si>
+  <si>
+    <t>Publicly available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains a range of topics including labour market and education by local authority. </t>
+  </si>
+  <si>
+    <t>ONS</t>
+  </si>
+  <si>
+    <t>Query labour market data at national, regional and local levels</t>
+  </si>
+  <si>
+    <t>https://www.nomisweb.co.uk/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publicly available, with more functionality if you create an account. </t>
+  </si>
+  <si>
+    <t>Explore Education Statistics</t>
+  </si>
+  <si>
+    <t>DfE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A range of educational data published by the Department of Education </t>
+  </si>
+  <si>
+    <t>https://explore-education-statistics.service.gov.uk/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publicly available </t>
+  </si>
+  <si>
+    <t>Lists useful data sources related to colleges</t>
+  </si>
+  <si>
+    <t>AoC</t>
+  </si>
+  <si>
+    <t>Working Futures 20235</t>
   </si>
 </sst>
 </file>
@@ -406,7 +472,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,21 +480,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455C0F38-06FA-4C4D-8065-41AFD4764DD8}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -445,7 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -457,6 +524,96 @@
       </c>
       <c r="E2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct a time comment issue updtae data sources to be links added in a load of data the overview page needed
</commit_message>
<xml_diff>
--- a/Data/18_FeSources/FeSources.xlsx
+++ b/Data/18_FeSources/FeSources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/hannah_cox_education_gov_uk/Documents/Documents/Projects/lsip_dashboard/Data/18_FeSources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/18_FeSources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7297E987-FB5B-4F30-A6A2-190410A21B14}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E73AF32-ACC0-415A-B99C-A46524F08D2B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1065" yWindow="1185" windowWidth="5400" windowHeight="2813" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,18 +71,9 @@
     <t>Association of Colleges (AoC)</t>
   </si>
   <si>
-    <t>https://www.ons.gov.uk/peoplepopulationandcommunity/wellbeing/articles/subnationalindicatorsexplorer/2022-01-06</t>
-  </si>
-  <si>
-    <t>https://www.aoc.co.uk/research-unit/data-sources</t>
-  </si>
-  <si>
     <t>Census</t>
   </si>
   <si>
-    <t>https://census.gov.uk/local-authorities</t>
-  </si>
-  <si>
     <t>NOMIS</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>Query labour market data at national, regional and local levels</t>
   </si>
   <si>
-    <t>https://www.nomisweb.co.uk/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Publicly available, with more functionality if you create an account. </t>
   </si>
   <si>
@@ -116,9 +104,6 @@
     <t xml:space="preserve">A range of educational data published by the Department of Education </t>
   </si>
   <si>
-    <t>https://explore-education-statistics.service.gov.uk/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Publicly available </t>
   </si>
   <si>
@@ -129,6 +114,21 @@
   </si>
   <si>
     <t>Working Futures 20235</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/peoplepopulationandcommunity/wellbeing/articles/subnationalindicatorsexplorer/2022-01-06'&gt;ONS&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.aoc.co.uk/research-unit/data-sources'&gt;AOC&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://census.gov.uk/local-authorities'&gt;Census&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/'&gt;Nomis&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/'&gt;EES&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -483,19 +483,19 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -512,7 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -526,94 +526,94 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to merge to commit
</commit_message>
<xml_diff>
--- a/Data/18_FeSources/FeSources.xlsx
+++ b/Data/18_FeSources/FeSources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/hannah_cox_education_gov_uk/Documents/Documents/Projects/lsip_dashboard/Data/18_FeSources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/18_FeSources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0BDD28A-F030-4D21-AB82-F93368626CC3}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E73AF32-ACC0-415A-B99C-A46524F08D2B}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,18 +71,9 @@
     <t>Association of Colleges (AoC)</t>
   </si>
   <si>
-    <t>https://www.ons.gov.uk/peoplepopulationandcommunity/wellbeing/articles/subnationalindicatorsexplorer/2022-01-06</t>
-  </si>
-  <si>
-    <t>https://www.aoc.co.uk/research-unit/data-sources</t>
-  </si>
-  <si>
     <t>Census</t>
   </si>
   <si>
-    <t>https://census.gov.uk/local-authorities</t>
-  </si>
-  <si>
     <t>NOMIS</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>Query labour market data at national, regional and local levels</t>
   </si>
   <si>
-    <t>https://www.nomisweb.co.uk/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Publicly available, with more functionality if you create an account. </t>
   </si>
   <si>
@@ -116,9 +104,6 @@
     <t xml:space="preserve">A range of educational data published by the Department of Education </t>
   </si>
   <si>
-    <t>https://explore-education-statistics.service.gov.uk/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Publicly available </t>
   </si>
   <si>
@@ -128,7 +113,22 @@
     <t>AoC</t>
   </si>
   <si>
-    <t>Working Futures 2035</t>
+    <t>Working Futures 20235</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/peoplepopulationandcommunity/wellbeing/articles/subnationalindicatorsexplorer/2022-01-06'&gt;ONS&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.aoc.co.uk/research-unit/data-sources'&gt;AOC&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://census.gov.uk/local-authorities'&gt;Census&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/'&gt;Nomis&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/'&gt;EES&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -483,19 +483,19 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -512,7 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -526,94 +526,94 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new source and tool tables
</commit_message>
<xml_diff>
--- a/Data/18_FeSources/FeSources.xlsx
+++ b/Data/18_FeSources/FeSources.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/18_FeSources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29411EF3-836C-4C74-A178-3A37661F96D8}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFABE57B-2773-493F-839D-BAA8D9030FC7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tools" sheetId="1" r:id="rId1"/>
+    <sheet name="Sources" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Source</t>
   </si>
@@ -101,23 +102,141 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/'&gt;EES&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Skills Imperative 2035</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.nuffieldfoundation.org/project/the-skills-imperative-2035'&gt;NFER&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href='https://census.gov.uk/local-authorities'&gt;ONS&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Report publicly available, data available soon</t>
+    <t>LA schools scorecard</t>
+  </si>
+  <si>
+    <t>Scorecards display a snapshot of the progress each local authority across England is making towards ensuring there are sufficient, good quality, school places.</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://department-for-education.shinyapps.io/la-school-places-scorecards/?_inputs_&amp;navbar=%22la_scorecards%22&amp;linkQuantityTab=0&amp;linkPreferenceTab=0&amp;phase_choice=%22Primary%22&amp;tabs_tech_notes=%22Quantity%22&amp;LA_choice=%22Barnet%22&amp;linkQualityTab=0&amp;tabs=%22cost%22&amp;linklascorecardsTab=0&amp;linkForecastTab=0&amp;linkCostTab=0'&gt;DfE&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Data​</t>
+  </si>
+  <si>
+    <t>Source​</t>
+  </si>
+  <si>
+    <t>Job quality indicator tables, UK by country, region and local authority</t>
+  </si>
+  <si>
+    <t>HE destination</t>
+  </si>
+  <si>
+    <t>Region of residence after HE</t>
+  </si>
+  <si>
+    <t>FE destination</t>
+  </si>
+  <si>
+    <t>Apprenticeship destination</t>
+  </si>
+  <si>
+    <t>Gross value added (GVA) per hour worked </t>
+  </si>
+  <si>
+    <t>Median wage</t>
+  </si>
+  <si>
+    <t>Population by age</t>
+  </si>
+  <si>
+    <t>Data showing the proportions of 16- and 17-year-olds in education and training and an estimate of those not in education, employment or training (NEET).</t>
+  </si>
+  <si>
+    <t>Employer Skills Survey including hard-to-fill and skill-shortage vacancies, employer skills needed in next 12 months, and percent opf employers providing training</t>
+  </si>
+  <si>
+    <t>Skills Imperative by LA, LSIP, LEP and MCA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Skills Imperative 2035 - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Coming soon</t>
+    </r>
+  </si>
+  <si>
+    <t>ONS Vacancies by SOC</t>
+  </si>
+  <si>
+    <t>Coming soon</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ESS 2023 - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Coming Summer 2024</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.beta.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/qualityworkcomponentandcompositetablesuk2018'&gt;Job quality indicator tables, UK - Office for National Statistics (ons.gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ethnicity-facts-figures.service.gov.uk/education-skills-and-training/after-education/destinations-and-earnings-of-graduates-after-higher-education/latest'&gt;Destinations and earnings of graduates after higher education - GOV.UK Ethnicity facts and figures (ethnicity-facts-figures.service.gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.hesa.ac.uk/news/16-06-2022/sb263-higher-education-graduate-outcomes-statistics/salary'&gt;Graduate Outcomes 2019/20: Summary Statistics - Graduate salaries and work locations | HESA&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/fast-track/b8aabe3c-5f3c-48b5-929c-8615d57d1d98'&gt;EES&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/further-education-outcome-based-success-measures'&gt;EES&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/labourproductivity/datasets/subregionalproductivitylabourproductivitygvaperhourworkedandgvaperfilledjobindicesbylocalenterprisepartnership'&gt;Subregional productivity: labour productivity indices by economic enterprise region - Office for National Statistics (ons.gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/ashe'&gt;ASHE Nomis&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/apsnew'&gt;APS Nomis&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.gov.uk/government/publications/neet-and-participation-local-authority-figures'&gt;NEET and participation: local authority figures - GOV.UK (www.gov.uk)&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,16 +244,74 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -142,14 +319,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455C0F38-06FA-4C4D-8065-41AFD4764DD8}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,15 +751,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
+    <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -520,13 +767,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -534,44 +781,170 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACE25F3-3BBD-4BFB-8DFC-B2B552BE112F}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new LAs to the KS5 data summarise it at the new LA level Force any areas with only one LA to not add LA map comment
</commit_message>
<xml_diff>
--- a/Data/18_FeSources/FeSources.xlsx
+++ b/Data/18_FeSources/FeSources.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/18_FeSources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\18_FeSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{2D3A2B6E-EAB5-4658-ABD9-7280747BA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFABE57B-2773-493F-839D-BAA8D9030FC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95969516-7F40-4D5D-BC33-B0C1D7498CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
@@ -147,9 +147,6 @@
     <t>Data showing the proportions of 16- and 17-year-olds in education and training and an estimate of those not in education, employment or training (NEET).</t>
   </si>
   <si>
-    <t>Employer Skills Survey including hard-to-fill and skill-shortage vacancies, employer skills needed in next 12 months, and percent opf employers providing training</t>
-  </si>
-  <si>
     <t>Skills Imperative by LA, LSIP, LEP and MCA</t>
   </si>
   <si>
@@ -180,6 +177,33 @@
     <t>Coming soon</t>
   </si>
   <si>
+    <t>&lt;a href='https://www.beta.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/qualityworkcomponentandcompositetablesuk2018'&gt;Job quality indicator tables, UK - Office for National Statistics (ons.gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ethnicity-facts-figures.service.gov.uk/education-skills-and-training/after-education/destinations-and-earnings-of-graduates-after-higher-education/latest'&gt;Destinations and earnings of graduates after higher education - GOV.UK Ethnicity facts and figures (ethnicity-facts-figures.service.gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.hesa.ac.uk/news/16-06-2022/sb263-higher-education-graduate-outcomes-statistics/salary'&gt;Graduate Outcomes 2019/20: Summary Statistics - Graduate salaries and work locations | HESA&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/fast-track/b8aabe3c-5f3c-48b5-929c-8615d57d1d98'&gt;EES&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/further-education-outcome-based-success-measures'&gt;EES&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/labourproductivity/datasets/subregionalproductivitylabourproductivitygvaperhourworkedandgvaperfilledjobindicesbylocalenterprisepartnership'&gt;Subregional productivity: labour productivity indices by economic enterprise region - Office for National Statistics (ons.gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/ashe'&gt;ASHE Nomis&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/apsnew'&gt;APS Nomis&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.gov.uk/government/publications/neet-and-participation-local-authority-figures'&gt;NEET and participation: local authority figures - GOV.UK (www.gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">ESS 2023 - </t>
     </r>
@@ -191,59 +215,18 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Coming Summer 2024</t>
+      <t>Coming Summer 2023</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.beta.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/qualityworkcomponentandcompositetablesuk2018'&gt;Job quality indicator tables, UK - Office for National Statistics (ons.gov.uk)&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.ethnicity-facts-figures.service.gov.uk/education-skills-and-training/after-education/destinations-and-earnings-of-graduates-after-higher-education/latest'&gt;Destinations and earnings of graduates after higher education - GOV.UK Ethnicity facts and figures (ethnicity-facts-figures.service.gov.uk)&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.hesa.ac.uk/news/16-06-2022/sb263-higher-education-graduate-outcomes-statistics/salary'&gt;Graduate Outcomes 2019/20: Summary Statistics - Graduate salaries and work locations | HESA&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/fast-track/b8aabe3c-5f3c-48b5-929c-8615d57d1d98'&gt;EES&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/further-education-outcome-based-success-measures'&gt;EES&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/labourproductivity/datasets/subregionalproductivitylabourproductivitygvaperhourworkedandgvaperfilledjobindicesbylocalenterprisepartnership'&gt;Subregional productivity: labour productivity indices by economic enterprise region - Office for National Statistics (ons.gov.uk)&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/ashe'&gt;ASHE Nomis&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/apsnew'&gt;APS Nomis&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.gov.uk/government/publications/neet-and-participation-local-authority-figures'&gt;NEET and participation: local authority figures - GOV.UK (www.gov.uk)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Employer Skills Survey including hard-to-fill and skill-shortage vacancies, employer skills needed in next 12 months, and percent of employers providing training</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,26 +346,26 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -391,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -831,7 +814,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -852,7 +835,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -860,7 +843,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -868,7 +851,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -876,7 +859,7 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -884,7 +867,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -892,7 +875,7 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -900,7 +883,7 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -908,7 +891,7 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
@@ -916,35 +899,35 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added in all the text for the skills iperative
</commit_message>
<xml_diff>
--- a/Data/18_FeSources/FeSources.xlsx
+++ b/Data/18_FeSources/FeSources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\18_FeSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95969516-7F40-4D5D-BC33-B0C1D7498CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1BA114-28D6-4E24-B455-9AD0080A627D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Source</t>
   </si>
@@ -145,30 +145,6 @@
   </si>
   <si>
     <t>Data showing the proportions of 16- and 17-year-olds in education and training and an estimate of those not in education, employment or training (NEET).</t>
-  </si>
-  <si>
-    <t>Skills Imperative by LA, LSIP, LEP and MCA</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Skills Imperative 2035 - </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Coming soon</t>
-    </r>
   </si>
   <si>
     <t>ONS Vacancies by SOC</t>
@@ -811,10 +787,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACE25F3-3BBD-4BFB-8DFC-B2B552BE112F}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -835,7 +811,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -843,7 +819,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -851,7 +827,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -859,7 +835,7 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -867,7 +843,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -875,7 +851,7 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -883,7 +859,7 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -891,7 +867,7 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
@@ -899,31 +875,23 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tody code add a few more tools add skills imp link
</commit_message>
<xml_diff>
--- a/Data/18_FeSources/FeSources.xlsx
+++ b/Data/18_FeSources/FeSources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\18_FeSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1BA114-28D6-4E24-B455-9AD0080A627D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D9A18D-45FD-479B-8496-973F64667A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A5D4C3F6-9CE9-44C0-BBBD-467D1E450A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Tools" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Source</t>
   </si>
@@ -196,6 +196,24 @@
   </si>
   <si>
     <t>Employer Skills Survey including hard-to-fill and skill-shortage vacancies, employer skills needed in next 12 months, and percent of employers providing training</t>
+  </si>
+  <si>
+    <t>Get data about people and the communities they live in, includes population, identity, housing, people in or out of work, education and health.</t>
+  </si>
+  <si>
+    <t>Experimental statistics release showing clustering analysis exploring similarities between local authorities in England</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/visualisations/areas/'&gt;ONS&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>ONS area information</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/peoplepopulationandcommunity/wellbeing/articles/clusteringlocalauthoritiesagainstsubnationalindicatorsengland/2023-02-24'&gt;ONS&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>ONS clustering local authorities</t>
   </si>
 </sst>
 </file>
@@ -668,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455C0F38-06FA-4C4D-8065-41AFD4764DD8}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,8 +798,37 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -789,7 +836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACE25F3-3BBD-4BFB-8DFC-B2B552BE112F}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>